<commit_message>
Configured Framework to write status values for each transaction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature_Workspace\uipath-automation-5\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD5D1DF-92EF-4B31-944D-FBA1555CA6F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51786AA8-C70E-4835-915E-D1264013DA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1410" windowWidth="27420" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -131,6 +131,33 @@
   </si>
   <si>
     <t>Kill process</t>
+  </si>
+  <si>
+    <t>Status_Success</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record successful transaction.</t>
+  </si>
+  <si>
+    <t>Status_Failure</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record failed transaction.</t>
+  </si>
+  <si>
+    <t>Status_Pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Status message for TransactionData to record pending transaction.</t>
   </si>
 </sst>
 </file>
@@ -508,16 +535,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -566,7 +593,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1591,14 +1618,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1635,7 +1664,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1717,9 +1746,39 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2705,12 +2764,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Updated BusinessProcessName in Config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrobw\Desktop\Revature\P3\uipath-automation-7\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPathBatch\Project_3\uipath-automation-7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E29A181-17CB-4393-9051-DA766B2DE3E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECBA445-A610-4FAF-93FE-220063842FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23910" yWindow="3030" windowWidth="19335" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>ProcessABCQueue</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Credential name to use to get GitHub login information. (Orchestrator and/or Windows Credential Manager)</t>
+  </si>
+  <si>
+    <t>ForkGithubRepository</t>
   </si>
 </sst>
 </file>
@@ -542,15 +542,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -589,49 +589,49 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="28.8">
+    <row r="4" spans="1:26" ht="29">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1638,12 +1638,12 @@
       <selection activeCell="A14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1680,7 +1680,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1712,7 +1712,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1734,7 +1734,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1745,7 +1745,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1756,7 +1756,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1764,35 +1764,35 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2780,12 +2780,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2796,7 +2796,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
updated Config to match HandleOutput branch (resolving merge)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPathBatch\Project_3\uipath-automation-7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9DF2FAC-97C8-4A01-8CB4-7A6AB3236515}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECBA445-A610-4FAF-93FE-220063842FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22320" yWindow="2640" windowWidth="19335" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23910" yWindow="3030" windowWidth="19335" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>ProcessABCQueue</t>
@@ -166,10 +163,7 @@
     <t>Credential name to use to get GitHub login information. (Orchestrator and/or Windows Credential Manager)</t>
   </si>
   <si>
-    <t>MicrosoftEdgeNewTab</t>
-  </si>
-  <si>
-    <t>edge://newtab/</t>
+    <t>ForkGithubRepository</t>
   </si>
 </sst>
 </file>
@@ -548,7 +542,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -595,13 +589,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -610,41 +604,34 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
-    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1701,7 +1688,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1725,7 +1712,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1747,7 +1734,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1758,7 +1745,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1769,7 +1756,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1777,35 +1764,35 @@
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>42</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -2809,7 +2796,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
updated Config to include edge new tab url
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPathBatch\Project_3\uipath-automation-7\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cito\Revature\UiPath Project 3\uipath-automation-7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECBA445-A610-4FAF-93FE-220063842FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F19F4A2-AD2B-4EC5-98EA-2A76A15AA28F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23910" yWindow="3030" windowWidth="19335" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>ForkGithubRepository</t>
+  </si>
+  <si>
+    <t>MicrosoftEdgeNewTab</t>
+  </si>
+  <si>
+    <t>edge://newtab/</t>
+  </si>
+  <si>
+    <t>Url for blank tab when opening Edge.</t>
   </si>
 </sst>
 </file>
@@ -215,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -225,6 +234,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,15 +552,15 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C14" sqref="B14:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -599,7 +609,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="29">
+    <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -622,7 +632,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
         <v>43</v>
@@ -1638,12 +1658,12 @@
       <selection activeCell="A14" sqref="A14:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1680,7 +1700,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="28.8">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2780,12 +2800,12 @@
       <selection activeCell="C2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.90625" customWidth="1"/>
-    <col min="2" max="2" width="30.08984375" customWidth="1"/>
-    <col min="3" max="3" width="60.36328125" customWidth="1"/>
-    <col min="4" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>